<commit_message>
MODIFIED According to task
</commit_message>
<xml_diff>
--- a/names.xlsx
+++ b/names.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spots\Desktop\NewContent\New folder\Task-JS-Email-Script\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohammad Almajdi\Development\Task-JS-Email-Script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{065CB0E3-2463-465E-B687-99249DFE0F4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8F1AED9-CBB5-4765-9EBF-70BE30C89A69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{14BA8181-9CE3-4AB3-98DF-BCCC615F1735}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{14BA8181-9CE3-4AB3-98DF-BCCC615F1735}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,12 +40,6 @@
     <t>Html</t>
   </si>
   <si>
-    <t>Your Name</t>
-  </si>
-  <si>
-    <t>Your Email</t>
-  </si>
-  <si>
     <t>John Doe</t>
   </si>
   <si>
@@ -62,6 +56,12 @@
   </si>
   <si>
     <t>CSS</t>
+  </si>
+  <si>
+    <t>Mohammad salah</t>
+  </si>
+  <si>
+    <t>msdalmajdi@hotmail.com</t>
   </si>
 </sst>
 </file>
@@ -106,11 +106,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -435,54 +432,54 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="310" zoomScaleNormal="310" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.140625" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.1796875" customWidth="1"/>
+    <col min="2" max="2" width="21.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="2">
-        <v>100</v>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1">
+        <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="3" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>80</v>
       </c>
     </row>
@@ -490,8 +487,9 @@
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{F8881740-2CAD-4C16-AFAB-B4126BB33A9F}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{4508F876-69EE-4013-9ED1-432AB55E0B28}"/>
+    <hyperlink ref="B1" r:id="rId3" xr:uid="{70EF6834-42DC-4EAF-8D1F-19047F8BE398}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>